<commit_message>
agents should now be marked as parents by using group.mark_as_in_relationship()
</commit_message>
<xml_diff>
--- a/Excel Files/seed.xlsx
+++ b/Excel Files/seed.xlsx
@@ -144,10 +144,10 @@
       <alignment horizontal="center" wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+      <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -453,14 +453,14 @@
   <dimension ref="A1:I23"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
   <cols>
     <col min="1" max="5" width="8.83203125" style="1"/>
-    <col min="6" max="6" width="11.5" style="4" customWidth="1"/>
-    <col min="7" max="9" width="8.83203125" style="4"/>
+    <col min="6" max="6" width="11.5" style="3" customWidth="1"/>
+    <col min="7" max="9" width="8.83203125" style="3"/>
     <col min="10" max="16384" width="8.83203125" style="1"/>
   </cols>
   <sheetData>
@@ -480,24 +480,24 @@
       <c r="E1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="F1" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2"/>
-      <c r="I1" s="2"/>
+      <c r="G1" s="4"/>
+      <c r="H1" s="4"/>
+      <c r="I1" s="4"/>
     </row>
     <row r="2" spans="1:9">
-      <c r="F2" s="3" t="s">
+      <c r="F2" s="2" t="s">
         <v>19</v>
       </c>
-      <c r="G2" s="3" t="s">
+      <c r="G2" s="2" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="3" t="s">
+      <c r="H2" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="I2" s="3" t="s">
+      <c r="I2" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -514,7 +514,7 @@
       <c r="D3" s="1">
         <v>1</v>
       </c>
-      <c r="F3" s="4">
+      <c r="F3" s="3">
         <v>15</v>
       </c>
     </row>
@@ -531,7 +531,7 @@
       <c r="D4" s="1">
         <v>1</v>
       </c>
-      <c r="F4" s="4">
+      <c r="F4" s="3">
         <v>16</v>
       </c>
     </row>
@@ -548,7 +548,7 @@
       <c r="D5" s="1">
         <v>1</v>
       </c>
-      <c r="F5" s="4">
+      <c r="F5" s="3">
         <v>12</v>
       </c>
     </row>
@@ -565,7 +565,7 @@
       <c r="D6" s="1">
         <v>2</v>
       </c>
-      <c r="F6" s="4">
+      <c r="F6" s="3">
         <v>14</v>
       </c>
     </row>
@@ -582,7 +582,7 @@
       <c r="D7" s="1">
         <v>3</v>
       </c>
-      <c r="F7" s="4">
+      <c r="F7" s="3">
         <v>16</v>
       </c>
     </row>
@@ -599,7 +599,7 @@
       <c r="D8" s="1">
         <v>4</v>
       </c>
-      <c r="F8" s="4">
+      <c r="F8" s="3">
         <v>18</v>
       </c>
     </row>
@@ -616,7 +616,7 @@
       <c r="D9" s="1">
         <v>2</v>
       </c>
-      <c r="F9" s="4">
+      <c r="F9" s="3">
         <v>17</v>
       </c>
     </row>
@@ -633,7 +633,7 @@
       <c r="D10" s="1">
         <v>2</v>
       </c>
-      <c r="F10" s="4">
+      <c r="F10" s="3">
         <v>15</v>
       </c>
     </row>
@@ -650,7 +650,7 @@
       <c r="D11" s="1">
         <v>2</v>
       </c>
-      <c r="F11" s="4">
+      <c r="F11" s="3">
         <v>13</v>
       </c>
     </row>
@@ -667,7 +667,7 @@
       <c r="D12" s="1">
         <v>3</v>
       </c>
-      <c r="F12" s="4">
+      <c r="F12" s="3">
         <v>17</v>
       </c>
     </row>
@@ -684,7 +684,7 @@
       <c r="D13" s="1">
         <v>6</v>
       </c>
-      <c r="H13" s="4">
+      <c r="H13" s="3">
         <v>19</v>
       </c>
     </row>
@@ -704,10 +704,10 @@
       <c r="E14" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="G14" s="4" t="s">
+      <c r="G14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="I14" s="4">
+      <c r="I14" s="3">
         <v>20</v>
       </c>
     </row>
@@ -724,7 +724,7 @@
       <c r="D15" s="1">
         <v>8</v>
       </c>
-      <c r="G15" s="4">
+      <c r="G15" s="3">
         <v>17</v>
       </c>
     </row>
@@ -741,10 +741,10 @@
       <c r="D16" s="1">
         <v>9</v>
       </c>
-      <c r="G16" s="4" t="s">
+      <c r="G16" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="I16" s="4">
+      <c r="I16" s="3">
         <v>21</v>
       </c>
     </row>
@@ -761,10 +761,10 @@
       <c r="D17" s="1">
         <v>16</v>
       </c>
-      <c r="G17" s="4">
+      <c r="G17" s="3">
         <v>16</v>
       </c>
-      <c r="I17" s="4">
+      <c r="I17" s="3">
         <v>17</v>
       </c>
     </row>
@@ -781,10 +781,10 @@
       <c r="D18" s="1">
         <v>19</v>
       </c>
-      <c r="G18" s="4">
+      <c r="G18" s="3">
         <v>15</v>
       </c>
-      <c r="I18" s="4" t="s">
+      <c r="I18" s="3" t="s">
         <v>25</v>
       </c>
     </row>
@@ -801,10 +801,10 @@
       <c r="D19" s="1">
         <v>20</v>
       </c>
-      <c r="G19" s="4">
+      <c r="G19" s="3">
         <v>13</v>
       </c>
-      <c r="I19" s="4" t="s">
+      <c r="I19" s="3" t="s">
         <v>26</v>
       </c>
     </row>
@@ -821,10 +821,10 @@
       <c r="D20" s="1">
         <v>25</v>
       </c>
-      <c r="G20" s="4" t="s">
+      <c r="G20" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="I20" s="4">
+      <c r="I20" s="3">
         <v>16</v>
       </c>
     </row>
@@ -841,7 +841,7 @@
       <c r="D21" s="1">
         <v>7</v>
       </c>
-      <c r="H21" s="4" t="s">
+      <c r="H21" s="3" t="s">
         <v>23</v>
       </c>
     </row>
@@ -858,10 +858,10 @@
       <c r="D22" s="1">
         <v>18</v>
       </c>
-      <c r="H22" s="4" t="s">
+      <c r="H22" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="I22" s="4">
+      <c r="I22" s="3">
         <v>12</v>
       </c>
     </row>
@@ -881,10 +881,10 @@
       <c r="E23" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H23" s="4">
+      <c r="H23" s="3">
         <v>20</v>
       </c>
-      <c r="I23" s="4">
+      <c r="I23" s="3">
         <v>14</v>
       </c>
     </row>

</xml_diff>